<commit_message>
Pequeño cambio esqueleto de guión
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion08/EsqueletoGuion_CN_06_08_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion08/EsqueletoGuion_CN_06_08_CO.xlsx
@@ -5,11 +5,11 @@
   <workbookPr autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\German\Documents\Aulaplaneta All\Trabajos de editor\EDITOR\Sofía CN_06_08_CO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\German\Documents\GitHub\CienciasNaturales\fuentes\contenidos\grado06\guion08\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="1395" windowWidth="12240" windowHeight="9240" tabRatio="729" activeTab="4"/>
+    <workbookView xWindow="3405" yWindow="1395" windowWidth="12240" windowHeight="9240" tabRatio="729" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'CUADERNO DE ESTUDIO'!$A$1:$I$146</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'RECURSOS NUEVOS'!$A$1:$C$22</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">'RECURSOS NUEVOS'!$A$1:$C$23</definedName>
   </definedNames>
   <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="755" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="93">
   <si>
     <t>FICHA</t>
   </si>
@@ -311,6 +311,9 @@
   </si>
   <si>
     <t xml:space="preserve">La selva húmeda tropical </t>
+  </si>
+  <si>
+    <t>Maoa conceptual</t>
   </si>
 </sst>
 </file>
@@ -1834,10 +1837,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D24"/>
+  <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2095,7 +2098,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>82</v>
+        <v>92</v>
       </c>
       <c r="B22" t="s">
         <v>21</v>
@@ -2106,13 +2109,25 @@
       <c r="D22" s="4"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>82</v>
+      </c>
+      <c r="B23" t="s">
+        <v>21</v>
+      </c>
+      <c r="C23">
+        <v>22</v>
+      </c>
       <c r="D23" s="4"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="D24" s="4"/>
     </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D25" s="4"/>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:C22"/>
+  <autoFilter ref="A1:C23"/>
   <sortState ref="A2:C65">
     <sortCondition ref="C2:C65"/>
   </sortState>
@@ -2131,10 +2146,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:C28"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B29" sqref="B29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2380,17 +2395,28 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>82</v>
+        <v>23</v>
       </c>
       <c r="C22" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C23"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="C28" s="6"/>
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" t="s">
+        <v>82</v>
+      </c>
+      <c r="C23" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C24"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C29" s="6"/>
     </row>
   </sheetData>
   <sortState ref="A2:C38">
@@ -2411,8 +2437,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X184"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="57" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="57" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Pequeño cambio esqueleto guión
</commit_message>
<xml_diff>
--- a/fuentes/contenidos/grado06/guion08/EsqueletoGuion_CN_06_08_CO.xlsx
+++ b/fuentes/contenidos/grado06/guion08/EsqueletoGuion_CN_06_08_CO.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="3405" yWindow="1395" windowWidth="12240" windowHeight="9240" tabRatio="729" activeTab="2"/>
+    <workbookView xWindow="3405" yWindow="1395" windowWidth="12240" windowHeight="9240" tabRatio="729" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="GUION" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="759" uniqueCount="92">
   <si>
     <t>FICHA</t>
   </si>
@@ -311,9 +311,6 @@
   </si>
   <si>
     <t xml:space="preserve">La selva húmeda tropical </t>
-  </si>
-  <si>
-    <t>Maoa conceptual</t>
   </si>
 </sst>
 </file>
@@ -1690,7 +1687,7 @@
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="110" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1839,8 +1836,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D25"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="A28" sqref="A27:A28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2098,7 +2095,7 @@
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>92</v>
+        <v>23</v>
       </c>
       <c r="B22" t="s">
         <v>21</v>
@@ -2149,7 +2146,7 @@
   <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView zoomScale="90" zoomScaleNormal="90" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2437,9 +2434,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X184"/>
   <sheetViews>
-    <sheetView zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="57" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A128" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
+    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" zoomScaleSheetLayoutView="57" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C145" sqref="C145"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>